<commit_message>
Added components to libs
</commit_message>
<xml_diff>
--- a/Schematic/Schematic_Component_Setup_Time_Study.xlsx
+++ b/Schematic/Schematic_Component_Setup_Time_Study.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Stop Time</t>
   </si>
   <si>
-    <t>Time Duration</t>
-  </si>
-  <si>
     <t>Goals</t>
   </si>
   <si>
@@ -49,6 +46,46 @@
   </si>
   <si>
     <t>USB2SERA10CFK</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>USB_Type_A_RA</t>
+  </si>
+  <si>
+    <t>Time Duration
+(HR:MIN)</t>
+  </si>
+  <si>
+    <t>Schematic</t>
+  </si>
+  <si>
+    <t>PCB Footprint</t>
+  </si>
+  <si>
+    <t>Test Point 5011</t>
+  </si>
+  <si>
+    <t>USB_Mini_AB_SMT</t>
+  </si>
+  <si>
+    <t>USB_Mini_B_SMT</t>
+  </si>
+  <si>
+    <t>USB_Mini_A_SMT</t>
+  </si>
+  <si>
+    <t>Switch_Rocker_SPDT_ON_ON</t>
+  </si>
+  <si>
+    <t>Electromechanical</t>
+  </si>
+  <si>
+    <t>Switch_Slide_DPDT_ON_ON</t>
+  </si>
+  <si>
+    <t>GRS-2012-2000_PTH</t>
   </si>
 </sst>
 </file>
@@ -56,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -110,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -120,13 +157,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,31 +480,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="7" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -464,24 +515,24 @@
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="7">
         <v>41142</v>
@@ -497,7 +548,218 @@
         <v>2.5000000000000022E-2</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7">
+        <v>41246</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="F3" s="5">
+        <f>E3-D3</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7">
+        <v>41246</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.64652777777777781</v>
+      </c>
+      <c r="F4" s="5">
+        <f>E4-D4</f>
+        <v>1.8055555555555602E-2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7">
+        <v>41246</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.64652777777777781</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.65486111111111112</v>
+      </c>
+      <c r="F5" s="5">
+        <f>E5-D5</f>
+        <v>8.3333333333333037E-3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="12">
+        <v>41246</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.65486111111111112</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.66527777777777775</v>
+      </c>
+      <c r="F6" s="9">
+        <f>E6-D6</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="7">
+        <v>41247</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="F9" s="5">
+        <f>E9-D9</f>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="7">
+        <v>41247</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="F10" s="5">
+        <f>E10-D10</f>
+        <v>4.8611111111111494E-3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="7">
+        <v>41247</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.4458333333333333</v>
+      </c>
+      <c r="F11" s="5">
+        <f>E11-D11</f>
+        <v>1.5277777777777724E-2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="D6:D8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>